<commit_message>
clean up and updated and modified EMPIRE version
</commit_message>
<xml_diff>
--- a/EMPIRE_extension/EMPIRE_input/Generator.xlsx
+++ b/EMPIRE_extension/EMPIRE_input/Generator.xlsx
@@ -21,6 +21,7 @@
     <sheet name="GeneratorTypeAvailability" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="CO2Content" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="Lifetime" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="OffshoreAreaMaxCapacity" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="arcs">#REF!</definedName>
@@ -13574,7 +13575,7 @@
       </c>
       <c r="C3" s="21" t="inlineStr">
         <is>
-          <t>generatorMaxInstallCapacity  in MW</t>
+          <t>generatorMaxInstallCapacity in MW</t>
         </is>
       </c>
       <c r="E3" s="25" t="n"/>
@@ -23492,6 +23493,347 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:B34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Node</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>offshoreWindAreaMaxInstallCapacity in MW</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Moray Firth</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>17110</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Firth of Forth</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>38275</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Dogger Bank</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>16260</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Hornsea</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>12055</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Outer Dowsing</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6265</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Norfolk</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>8130</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>East Anglia</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6755</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Borssele</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4881.916666666667</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Hollandsee Kust</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6664.166666666666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Helgoländer Bucht</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>22910.625</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Nordsøen</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20110</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nordvest A</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>56535</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Nordvest C</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>27910</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Vestavind A</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>9420</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sønnavind A</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sørvest C</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>8830</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Nordvest B</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>17185</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Vestavind F</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>9945</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Vestavind B</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>14925</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Vestavind C</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>5320</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Vestavind D</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3670</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sørvest F</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>13510</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Sørvest B</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>10895</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Nordavind B</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>11195</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Nordavind A</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>21375</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Nordavind D</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>20560</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Nordavind C</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>5270</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Vestavind E</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>7375</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Sørvest E</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>5080</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Sørvest A</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>7280</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Sørvest D</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>6075</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>